<commit_message>
adicionado menu de selecao 21-03-25
</commit_message>
<xml_diff>
--- a/tipo_aco.xlsx
+++ b/tipo_aco.xlsx
@@ -82,6 +82,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -141,8 +142,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -272,301 +277,301 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>250</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>400</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>230</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>310</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>290</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>400</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="0" t="n">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>290</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>415</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="0" t="n">
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>345</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>450</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="0" t="n">
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>380</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>485</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="0" t="n">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>415</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>520</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="0" t="n">
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>450</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>550</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="0" t="s">
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>345</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>450</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>345</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>485</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="0" t="s">
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>315</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>460</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="0" t="s">
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>290</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>435</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="0" t="s">
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>345</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>485</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="0" t="n">
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>345</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>450</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="0" t="n">
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>415</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>520</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="0" t="n">
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>450</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>550</v>
       </c>
     </row>

</xml_diff>

<commit_message>
editando menu editar 23-03-25
</commit_message>
<xml_diff>
--- a/tipo_aco.xlsx
+++ b/tipo_aco.xlsx
@@ -20,17 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t xml:space="preserve">Tipo</t>
   </si>
   <si>
-    <t xml:space="preserve">Produto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grau</t>
-  </si>
-  <si>
     <t xml:space="preserve">fy</t>
   </si>
   <si>
@@ -40,22 +34,10 @@
     <t xml:space="preserve">ASTM A36</t>
   </si>
   <si>
-    <t xml:space="preserve">Perfis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
     <t xml:space="preserve">ASTM A500 GRAU A</t>
   </si>
   <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
     <t xml:space="preserve">ASTM A500 GRAU B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
   </si>
   <si>
     <t xml:space="preserve">ASTM A572 GRAU 42</t>
@@ -295,10 +277,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -317,282 +299,180 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>250</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="C2" s="1" t="n">
         <v>400</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>230</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="C3" s="1" t="n">
         <v>310</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>290</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="C4" s="1" t="n">
         <v>400</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B5" s="1" t="n">
+        <v>290</v>
+      </c>
       <c r="C5" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>290</v>
-      </c>
-      <c r="E5" s="1" t="n">
         <v>415</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>345</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>345</v>
-      </c>
-      <c r="E6" s="1" t="n">
         <v>450</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>380</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>380</v>
-      </c>
-      <c r="E7" s="1" t="n">
         <v>485</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>415</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>415</v>
-      </c>
-      <c r="E8" s="1" t="n">
         <v>520</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>450</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>450</v>
-      </c>
-      <c r="E9" s="1" t="n">
         <v>550</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="n">
         <v>345</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="C10" s="1" t="n">
         <v>450</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="n">
         <v>345</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="C11" s="1" t="n">
         <v>485</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="n">
         <v>315</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="C12" s="1" t="n">
         <v>460</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="n">
         <v>290</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="C13" s="1" t="n">
         <v>435</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="n">
         <v>345</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="C14" s="1" t="n">
         <v>485</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>345</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>345</v>
-      </c>
-      <c r="E15" s="1" t="n">
         <v>450</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>415</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>415</v>
-      </c>
-      <c r="E16" s="1" t="n">
         <v>520</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>450</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>450</v>
-      </c>
-      <c r="E17" s="1" t="n">
         <v>550</v>
       </c>
     </row>

</xml_diff>